<commit_message>
Updated 3D Print files
Added missing STLs for brackets and updated print files for chopsticks
gripper
</commit_message>
<xml_diff>
--- a/Bento Arm - 3D Printing Guide.xlsx
+++ b/Bento Arm - 3D Printing Guide.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rory\Dropbox\BLINC\Projects\BLINCdev\Repositories\Bento Arm Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rory\Documents\GitHub\Bento-Arm-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="170">
   <si>
     <t>Bento Arm V2 3D printed Part List</t>
   </si>
@@ -563,6 +563,12 @@
   <si>
     <t>QTY:1  - wrist_lateral_mount_rev3
 QTY:1 - wrist_medial_mount_rev3</t>
+  </si>
+  <si>
+    <t>Note2: Recommended print material for all parts is makerbot PLA</t>
+  </si>
+  <si>
+    <t>chopsticks_allparts_rev2b</t>
   </si>
 </sst>
 </file>
@@ -1309,217 +1315,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
-    <col min="8" max="8" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I20" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="14">
-        <v>145</v>
-      </c>
-      <c r="G20" s="14">
-        <v>32</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>24</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>31</v>
+      <c r="C21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="F21" s="14">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="G21" s="14">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="14">
+        <v>27</v>
+      </c>
+      <c r="G22" s="14">
+        <v>6</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="14">
-        <v>14</v>
-      </c>
-      <c r="G22" s="14">
-        <v>3</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
-        <v>29</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>32</v>
+      <c r="C23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="14">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G23" s="14">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>33</v>
+      <c r="C24" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="14">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G24" s="14">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>23</v>
@@ -1528,27 +1510,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>38</v>
+      <c r="C25" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="14">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="G25" s="14">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>23</v>
@@ -1557,27 +1539,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>83</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="14">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="G26" s="14">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>23</v>
@@ -1586,27 +1568,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>83</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="14">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G27" s="14">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>23</v>
@@ -1615,114 +1597,114 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>83</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="14">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="G28" s="14">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>23</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>161</v>
+        <v>50</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="F29" s="14">
-        <v>190</v>
+        <v>51</v>
       </c>
       <c r="G29" s="14">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>23</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>80</v>
+        <v>169</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>81</v>
+        <v>161</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="F30" s="14">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="G30" s="14">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>23</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>85</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="F31" s="14">
-        <v>22</v>
+        <v>150</v>
       </c>
       <c r="G31" s="14">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>23</v>
@@ -1731,56 +1713,56 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>116</v>
+        <v>85</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F32" s="14">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="G32" s="14">
+        <v>5</v>
+      </c>
+      <c r="H32" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>115</v>
       </c>
       <c r="I32" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F33" s="14">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="G33" s="14">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>115</v>
@@ -1789,27 +1771,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F34" s="14">
-        <v>115</v>
+        <v>157</v>
       </c>
       <c r="G34" s="14">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>115</v>
@@ -1818,27 +1800,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F35" s="14">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="G35" s="14">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>115</v>
@@ -1847,27 +1829,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F36" s="14">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="G36" s="14">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>115</v>
@@ -1876,27 +1858,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F37" s="14">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="G37" s="14">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>115</v>
@@ -1905,27 +1887,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F38" s="14">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="G38" s="14">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="H38" s="12" t="s">
         <v>115</v>
@@ -1934,18 +1916,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>114</v>
@@ -1954,7 +1936,7 @@
         <v>55</v>
       </c>
       <c r="G39" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H39" s="12" t="s">
         <v>115</v>
@@ -1963,27 +1945,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>167</v>
+        <v>100</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F40" s="14">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="G40" s="14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>115</v>
@@ -1992,25 +1974,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D41" s="11"/>
+        <v>166</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>167</v>
+      </c>
       <c r="E41" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F41" s="14">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="G41" s="14">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>115</v>
@@ -2019,27 +2003,25 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>113</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F42" s="14">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="G42" s="14">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>115</v>
@@ -2048,27 +2030,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F43" s="14">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="G43" s="14">
-        <v>7.75</v>
+        <v>16</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>115</v>
@@ -2077,27 +2059,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>137</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>114</v>
       </c>
       <c r="F44" s="14">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G44" s="14">
-        <v>9.23</v>
+        <v>7.75</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>115</v>
@@ -2106,134 +2088,136 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
-    </row>
-    <row r="46" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="18" t="s">
+    <row r="45" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="14">
+        <v>37</v>
+      </c>
+      <c r="G45" s="14">
+        <v>9.23</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="H47" s="8"/>
-    </row>
-    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E49" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="G49" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+    <row r="50" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="4">
-        <v>1</v>
-      </c>
-      <c r="E49" s="4">
-        <v>28</v>
-      </c>
-      <c r="F49" s="4">
-        <f xml:space="preserve"> D49*E49</f>
-        <v>28</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4">
+        <v>28</v>
+      </c>
+      <c r="F50" s="4">
+        <f xml:space="preserve"> D50*E50</f>
+        <v>28</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="E50" s="4">
-        <v>1</v>
-      </c>
-      <c r="F50" s="4">
-        <f t="shared" ref="F50:F101" si="0" xml:space="preserve"> D50*E50</f>
-        <v>2</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D51" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F51" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>3</v>
+        <f t="shared" ref="F51:F102" si="0" xml:space="preserve"> D51*E51</f>
+        <v>2</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>83</v>
@@ -2242,52 +2226,52 @@
         <v>8</v>
       </c>
       <c r="D52" s="4">
+        <v>1</v>
+      </c>
+      <c r="E52" s="4">
         <v>4</v>
       </c>
-      <c r="E52" s="4">
-        <v>0.5</v>
-      </c>
       <c r="F52" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D53" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E53" s="4">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="F53" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G53" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>83</v>
@@ -2299,49 +2283,49 @@
         <v>1</v>
       </c>
       <c r="E54" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
       </c>
       <c r="E55" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F55" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G55" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>83</v>
@@ -2350,25 +2334,25 @@
         <v>8</v>
       </c>
       <c r="D56" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E56" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F56" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>39</v>
+        <v>4</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>83</v>
@@ -2377,52 +2361,52 @@
         <v>8</v>
       </c>
       <c r="D57" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D58" s="4">
         <v>1</v>
       </c>
       <c r="E58" s="4">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F58" s="4">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>83</v>
@@ -2434,71 +2418,76 @@
         <v>1</v>
       </c>
       <c r="E59" s="4">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F59" s="4">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="4">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4">
+        <v>27</v>
+      </c>
+      <c r="F60" s="4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="4">
-        <v>1</v>
-      </c>
-      <c r="E60" s="4">
+      <c r="D61" s="4">
+        <v>1</v>
+      </c>
+      <c r="E61" s="4">
         <v>10</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F61" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="4">
-        <v>1</v>
-      </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>145</v>
@@ -2512,15 +2501,15 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>145</v>
@@ -2534,15 +2523,15 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>145</v>
@@ -2556,15 +2545,15 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>145</v>
@@ -2573,43 +2562,42 @@
         <v>8</v>
       </c>
       <c r="D65" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="4">
+        <v>2</v>
+      </c>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" s="4">
-        <v>1</v>
-      </c>
-      <c r="E66" s="4">
-        <v>196</v>
-      </c>
-      <c r="F66" s="4">
-        <f t="shared" si="0"/>
-        <v>196</v>
-      </c>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>84</v>
@@ -2621,18 +2609,18 @@
         <v>1</v>
       </c>
       <c r="E67" s="4">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F67" s="4">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>84</v>
@@ -2644,18 +2632,18 @@
         <v>1</v>
       </c>
       <c r="E68" s="4">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F68" s="4">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>84</v>
@@ -2667,18 +2655,18 @@
         <v>1</v>
       </c>
       <c r="E69" s="4">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="F69" s="4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>84</v>
@@ -2690,18 +2678,18 @@
         <v>1</v>
       </c>
       <c r="E70" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" s="4">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>84</v>
@@ -2713,64 +2701,64 @@
         <v>1</v>
       </c>
       <c r="E71" s="4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F71" s="4">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="D72" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E72" s="4">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F72" s="4">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="D73" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E73" s="4">
-        <v>159</v>
+        <v>4</v>
       </c>
       <c r="F73" s="4">
         <f t="shared" si="0"/>
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>84</v>
@@ -2781,17 +2769,19 @@
       <c r="D74" s="4">
         <v>1</v>
       </c>
-      <c r="E74" s="4"/>
+      <c r="E74" s="4">
+        <v>159</v>
+      </c>
       <c r="F74" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>84</v>
@@ -2800,47 +2790,41 @@
         <v>7</v>
       </c>
       <c r="D75" s="4">
-        <v>2</v>
-      </c>
-      <c r="E75" s="4">
-        <v>80</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E75" s="4"/>
       <c r="F75" s="4">
         <f t="shared" si="0"/>
-        <v>160</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E76" s="4">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="F76" s="4">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="G76" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>85</v>
@@ -2852,22 +2836,22 @@
         <v>1</v>
       </c>
       <c r="E77" s="4">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F77" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>85</v>
@@ -2886,15 +2870,15 @@
         <v>7</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>85</v>
@@ -2906,22 +2890,22 @@
         <v>1</v>
       </c>
       <c r="E79" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F79" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>85</v>
@@ -2930,25 +2914,25 @@
         <v>7</v>
       </c>
       <c r="D80" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E80" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F80" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>85</v>
@@ -2957,25 +2941,25 @@
         <v>7</v>
       </c>
       <c r="D81" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E81" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F81" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G81" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>85</v>
@@ -2984,25 +2968,25 @@
         <v>7</v>
       </c>
       <c r="D82" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E82" s="4">
         <v>0.25</v>
       </c>
       <c r="F82" s="4">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>85</v>
@@ -3011,50 +2995,50 @@
         <v>7</v>
       </c>
       <c r="D83" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E83" s="4">
         <v>0.25</v>
       </c>
       <c r="F83" s="4">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D84" s="4">
         <v>1</v>
       </c>
       <c r="E84" s="4">
-        <v>24</v>
+        <v>0.25</v>
       </c>
       <c r="F84" s="4">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>0.25</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>88</v>
       </c>
@@ -3062,53 +3046,53 @@
         <v>91</v>
       </c>
       <c r="C85" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D85" s="4">
+        <v>1</v>
+      </c>
+      <c r="E85" s="4">
+        <v>24</v>
+      </c>
+      <c r="F85" s="4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D85" s="4">
-        <v>1</v>
-      </c>
-      <c r="E85" s="4">
+      <c r="D86" s="4">
+        <v>1</v>
+      </c>
+      <c r="E86" s="4">
         <v>42</v>
       </c>
-      <c r="F85" s="4">
+      <c r="F86" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="G85" s="3" t="s">
+      <c r="G86" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="H86" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B86" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D86" s="14">
-        <v>1</v>
-      </c>
-      <c r="E86" s="14">
-        <v>2</v>
-      </c>
-      <c r="F86" s="14">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G86" t="s">
-        <v>92</v>
-      </c>
-      <c r="H86" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>88</v>
       </c>
@@ -3116,7 +3100,7 @@
         <v>91</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D87" s="14">
         <v>1</v>
@@ -3128,14 +3112,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G87" s="13" t="s">
-        <v>98</v>
+      <c r="G87" t="s">
+        <v>92</v>
       </c>
       <c r="H87" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>88</v>
       </c>
@@ -3143,7 +3127,7 @@
         <v>91</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D88" s="14">
         <v>1</v>
@@ -3156,40 +3140,40 @@
         <v>2</v>
       </c>
       <c r="G88" s="13" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H88" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B89" s="3" t="s">
+    <row r="89" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D89" s="4">
-        <v>1</v>
-      </c>
-      <c r="E89" s="4">
-        <v>19</v>
-      </c>
-      <c r="F89" s="4">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D89" s="14">
+        <v>1</v>
+      </c>
+      <c r="E89" s="14">
+        <v>2</v>
+      </c>
+      <c r="F89" s="14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G89" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H89" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>103</v>
       </c>
@@ -3197,26 +3181,26 @@
         <v>91</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D90" s="4">
         <v>1</v>
       </c>
       <c r="E90" s="4">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F90" s="4">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>103</v>
       </c>
@@ -3224,26 +3208,26 @@
         <v>91</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D91" s="4">
         <v>1</v>
       </c>
       <c r="E91" s="4">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F91" s="4">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>103</v>
       </c>
@@ -3251,26 +3235,26 @@
         <v>91</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D92" s="4">
         <v>1</v>
       </c>
       <c r="E92" s="4">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F92" s="4">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>103</v>
       </c>
@@ -3278,26 +3262,26 @@
         <v>91</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D93" s="4">
         <v>1</v>
       </c>
       <c r="E93" s="4">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F93" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>103</v>
       </c>
@@ -3305,7 +3289,7 @@
         <v>91</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D94" s="4">
         <v>1</v>
@@ -3318,13 +3302,13 @@
         <v>4</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>103</v>
       </c>
@@ -3332,26 +3316,26 @@
         <v>91</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D95" s="4">
         <v>1</v>
       </c>
       <c r="E95" s="4">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="F95" s="4">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>103</v>
       </c>
@@ -3359,7 +3343,7 @@
         <v>91</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D96" s="4">
         <v>1</v>
@@ -3372,13 +3356,13 @@
         <v>0.5</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>103</v>
       </c>
@@ -3386,26 +3370,26 @@
         <v>91</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D97" s="4">
         <v>1</v>
       </c>
       <c r="E97" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F97" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>103</v>
       </c>
@@ -3413,7 +3397,7 @@
         <v>91</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D98" s="4">
         <v>1</v>
@@ -3426,13 +3410,13 @@
         <v>2</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H98" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
@@ -3440,7 +3424,7 @@
         <v>91</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D99" s="4">
         <v>1</v>
@@ -3453,13 +3437,13 @@
         <v>2</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H99" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>103</v>
       </c>
@@ -3467,7 +3451,7 @@
         <v>91</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D100" s="4">
         <v>1</v>
@@ -3480,24 +3464,51 @@
         <v>2</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H100" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="3"/>
+    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D101" s="4">
+        <v>1</v>
+      </c>
+      <c r="E101" s="4">
+        <v>2</v>
+      </c>
       <c r="F101" s="4">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H101" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated arm shells, electronics enclosure, and documentation with minor improvements
- updated assembly guide, bill of materials, and electronics
wiring/cabling diagram to reflect a change to a SPST on/off switch
- added more detailed section in assembly guide on how to make the arm
shells
- Added more material to the wrist arm shell mounts.
- Adjusted the magnet mounts, so that the magnets will sit a bit closer
to the tops of the screws to give better adhesion
- Removed material from enclosure_body_rev3, so that the DIN 8 connector
can fit through the on/off switch cutout
</commit_message>
<xml_diff>
--- a/Bento Arm - 3D Printing Guide.xlsx
+++ b/Bento Arm - 3D Printing Guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="171">
   <si>
     <t>Bento Arm V2 3D printed Part List</t>
   </si>
@@ -270,13 +270,6 @@
   </si>
   <si>
     <t>enclosure_all_rev3</t>
-  </si>
-  <si>
-    <t>QTY:1 - enclosure_body_rev3
-QTY:1 - enclosure_lid_back_rev2
-QTY:1 - enclosure_lid_front_rev2
-QTY:1 - cable _relief
-QTY:2 - molex bracket</t>
   </si>
   <si>
     <t>QTY:4 - cable_router_nut_PLA
@@ -552,23 +545,39 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>magnet_armshell_mounts_rev3</t>
-  </si>
-  <si>
     <t>magnet_armshell_mounts</t>
   </si>
   <si>
-    <t>wrist_mounts_rev3</t>
-  </si>
-  <si>
-    <t>QTY:1  - wrist_lateral_mount_rev3
-QTY:1 - wrist_medial_mount_rev3</t>
-  </si>
-  <si>
     <t>Note2: Recommended print material for all parts is makerbot PLA</t>
   </si>
   <si>
     <t>chopsticks_allparts_rev2b</t>
+  </si>
+  <si>
+    <t>QTY:1 - enclosure_body_rev3_PLA
+QTY:1 - enclosure_lid_back_rev2_PLA
+QTY:1 - enclosure_lid_front_rev2_PLA
+QTY:1 - cable _relief_PLA
+QTY:2 - molex bracket_PLA</t>
+  </si>
+  <si>
+    <t>QTY:1 forearm_ventral_dist_mount_rev4
+QTY:1 forearm_ventral_prox_mount_rev4
+QTY:1 forearm_dorsal_dist_mount_rev4
+QTY:1 forearm_dorsal_prox_mount_rev4
+QTY:1 upper_dorsal_dist_mount_rev4
+QTY:1 upper_dorsal_prox_mount_rev4
+QTY:1 upper_ventral_mount_rev4</t>
+  </si>
+  <si>
+    <t>wrist_mounts_rev3b</t>
+  </si>
+  <si>
+    <t>magnet_armshell_mounts_rev4</t>
+  </si>
+  <si>
+    <t>QTY:1  - wrist_lateral_mount_rev3b
+QTY:1 - wrist_medial_mount_rev3b</t>
   </si>
 </sst>
 </file>
@@ -1317,15 +1326,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
@@ -1349,12 +1358,12 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1399,7 +1408,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>21</v>
@@ -1428,7 +1437,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>27</v>
@@ -1437,7 +1446,7 @@
         <v>31</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F22" s="14">
         <v>27</v>
@@ -1457,7 +1466,7 @@
         <v>56</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>56</v>
@@ -1486,7 +1495,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>29</v>
@@ -1515,7 +1524,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>33</v>
@@ -1544,7 +1553,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>36</v>
@@ -1573,7 +1582,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>44</v>
@@ -1602,7 +1611,7 @@
         <v>46</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>45</v>
@@ -1631,7 +1640,7 @@
         <v>51</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>50</v>
@@ -1657,19 +1666,19 @@
     </row>
     <row r="30" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D30" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="F30" s="14">
         <v>190</v>
@@ -1681,7 +1690,7 @@
         <v>23</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1689,13 +1698,13 @@
         <v>78</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>80</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>1</v>
@@ -1704,7 +1713,7 @@
         <v>150</v>
       </c>
       <c r="G31" s="14">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>23</v>
@@ -1718,16 +1727,16 @@
         <v>79</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>79</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F32" s="14">
         <v>22</v>
@@ -1744,19 +1753,19 @@
     </row>
     <row r="33" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F33" s="14">
         <v>105</v>
@@ -1765,7 +1774,7 @@
         <v>23</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>23</v>
@@ -1773,19 +1782,19 @@
     </row>
     <row r="34" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F34" s="14">
         <v>157</v>
@@ -1794,7 +1803,7 @@
         <v>43</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>23</v>
@@ -1802,19 +1811,19 @@
     </row>
     <row r="35" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35" s="14">
         <v>115</v>
@@ -1823,7 +1832,7 @@
         <v>19</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>23</v>
@@ -1831,19 +1840,19 @@
     </row>
     <row r="36" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="14">
         <v>60</v>
@@ -1852,7 +1861,7 @@
         <v>16</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>23</v>
@@ -1860,19 +1869,19 @@
     </row>
     <row r="37" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F37" s="14">
         <v>104</v>
@@ -1881,7 +1890,7 @@
         <v>29</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I37" s="12" t="s">
         <v>23</v>
@@ -1889,19 +1898,19 @@
     </row>
     <row r="38" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F38" s="14">
         <v>73</v>
@@ -1910,7 +1919,7 @@
         <v>19</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I38" s="12" t="s">
         <v>23</v>
@@ -1918,19 +1927,19 @@
     </row>
     <row r="39" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F39" s="14">
         <v>55</v>
@@ -1939,7 +1948,7 @@
         <v>5</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>23</v>
@@ -1947,19 +1956,19 @@
     </row>
     <row r="40" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F40" s="14">
         <v>55</v>
@@ -1968,7 +1977,7 @@
         <v>6</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I40" s="12" t="s">
         <v>23</v>
@@ -1976,28 +1985,28 @@
     </row>
     <row r="41" spans="1:9" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F41" s="14">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G41" s="14">
         <v>2</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I41" s="12" t="s">
         <v>23</v>
@@ -2005,26 +2014,28 @@
     </row>
     <row r="42" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42" s="11"/>
+        <v>163</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>167</v>
+      </c>
       <c r="E42" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="14">
+        <v>90</v>
+      </c>
+      <c r="G42" s="14">
+        <v>17</v>
+      </c>
+      <c r="H42" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="F42" s="14">
-        <v>86</v>
-      </c>
-      <c r="G42" s="14">
-        <v>20</v>
-      </c>
-      <c r="H42" s="12" t="s">
-        <v>115</v>
       </c>
       <c r="I42" s="12" t="s">
         <v>23</v>
@@ -2032,19 +2043,19 @@
     </row>
     <row r="43" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D43" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="F43" s="14">
         <v>72</v>
@@ -2053,7 +2064,7 @@
         <v>16</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I43" s="12" t="s">
         <v>23</v>
@@ -2061,19 +2072,19 @@
     </row>
     <row r="44" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="C44" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>138</v>
-      </c>
       <c r="E44" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F44" s="14">
         <v>31</v>
@@ -2082,7 +2093,7 @@
         <v>7.75</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I44" s="12" t="s">
         <v>23</v>
@@ -2090,19 +2101,19 @@
     </row>
     <row r="45" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C45" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>142</v>
-      </c>
       <c r="E45" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F45" s="14">
         <v>37</v>
@@ -2111,7 +2122,7 @@
         <v>9.23</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I45" s="12" t="s">
         <v>23</v>
@@ -2131,7 +2142,7 @@
     <row r="47" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H48" s="8"/>
     </row>
@@ -2166,7 +2177,7 @@
         <v>9</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>6</v>
@@ -2193,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>7</v>
@@ -2220,7 +2231,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>8</v>
@@ -2247,7 +2258,7 @@
         <v>54</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>8</v>
@@ -2274,7 +2285,7 @@
         <v>29</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>6</v>
@@ -2301,7 +2312,7 @@
         <v>33</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>6</v>
@@ -2328,7 +2339,7 @@
         <v>35</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>8</v>
@@ -2355,7 +2366,7 @@
         <v>39</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>8</v>
@@ -2382,7 +2393,7 @@
         <v>40</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>8</v>
@@ -2409,7 +2420,7 @@
         <v>41</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>42</v>
@@ -2436,7 +2447,7 @@
         <v>49</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>42</v>
@@ -2463,7 +2474,7 @@
         <v>51</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>7</v>
@@ -2487,10 +2498,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>8</v>
@@ -2501,18 +2512,18 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>8</v>
@@ -2523,18 +2534,18 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>8</v>
@@ -2545,18 +2556,18 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>8</v>
@@ -2567,18 +2578,18 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>8</v>
@@ -2589,10 +2600,10 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2600,7 +2611,7 @@
         <v>53</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>7</v>
@@ -2623,7 +2634,7 @@
         <v>58</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>7</v>
@@ -2646,7 +2657,7 @@
         <v>59</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>7</v>
@@ -2669,7 +2680,7 @@
         <v>60</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>7</v>
@@ -2692,7 +2703,7 @@
         <v>61</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>7</v>
@@ -2715,7 +2726,7 @@
         <v>62</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>7</v>
@@ -2738,7 +2749,7 @@
         <v>63</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>77</v>
@@ -2761,7 +2772,7 @@
         <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>7</v>
@@ -2784,7 +2795,7 @@
         <v>67</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>7</v>
@@ -2805,7 +2816,7 @@
         <v>68</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>7</v>
@@ -2827,7 +2838,7 @@
         <v>69</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>7</v>
@@ -2854,7 +2865,7 @@
         <v>70</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>7</v>
@@ -2881,7 +2892,7 @@
         <v>71</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>7</v>
@@ -2908,7 +2919,7 @@
         <v>72</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>7</v>
@@ -2935,7 +2946,7 @@
         <v>73</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>7</v>
@@ -2962,7 +2973,7 @@
         <v>74</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>7</v>
@@ -2989,7 +3000,7 @@
         <v>75</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>7</v>
@@ -3016,7 +3027,7 @@
         <v>76</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>7</v>
@@ -3040,13 +3051,13 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D85" s="4">
         <v>1</v>
@@ -3059,21 +3070,21 @@
         <v>24</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D86" s="4">
         <v>1</v>
@@ -3086,21 +3097,21 @@
         <v>42</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D87" s="14">
         <v>1</v>
@@ -3113,21 +3124,21 @@
         <v>2</v>
       </c>
       <c r="G87" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D88" s="14">
         <v>1</v>
@@ -3140,21 +3151,21 @@
         <v>2</v>
       </c>
       <c r="G88" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D89" s="14">
         <v>1</v>
@@ -3167,21 +3178,21 @@
         <v>2</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D90" s="4">
         <v>1</v>
@@ -3194,21 +3205,21 @@
         <v>19</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D91" s="4">
         <v>1</v>
@@ -3221,21 +3232,21 @@
         <v>16</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D92" s="4">
         <v>1</v>
@@ -3248,21 +3259,21 @@
         <v>29</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D93" s="4">
         <v>1</v>
@@ -3275,21 +3286,21 @@
         <v>19</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D94" s="4">
         <v>1</v>
@@ -3302,21 +3313,21 @@
         <v>4</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D95" s="4">
         <v>1</v>
@@ -3329,21 +3340,21 @@
         <v>4</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D96" s="4">
         <v>1</v>
@@ -3356,21 +3367,21 @@
         <v>0.5</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D97" s="4">
         <v>1</v>
@@ -3383,21 +3394,21 @@
         <v>0.5</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D98" s="4">
         <v>1</v>
@@ -3410,21 +3421,21 @@
         <v>2</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D99" s="4">
         <v>1</v>
@@ -3437,21 +3448,21 @@
         <v>2</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D100" s="4">
         <v>1</v>
@@ -3464,21 +3475,21 @@
         <v>2</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D101" s="4">
         <v>1</v>
@@ -3491,10 +3502,10 @@
         <v>2</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H101" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>